<commit_message>
Allow empty tag field and other space-based variations
(and test it in tiny)
</commit_message>
<xml_diff>
--- a/samples/tiny/config.xlsx
+++ b/samples/tiny/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="131">
   <si>
     <t xml:space="preserve">variables</t>
   </si>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">files_site</t>
   </si>
   <si>
-    <t xml:space="preserve">files_start</t>
+    <t xml:space="preserve">files_start (utc)</t>
   </si>
   <si>
     <t xml:space="preserve">files_tags</t>
@@ -101,6 +101,9 @@
     <t xml:space="preserve">all,band1</t>
   </si>
   <si>
+    <t xml:space="preserve">full</t>
+  </si>
+  <si>
     <t xml:space="preserve">log1,log2</t>
   </si>
   <si>
@@ -209,6 +212,9 @@
     <t xml:space="preserve">20210429_181000</t>
   </si>
   <si>
+    <t xml:space="preserve">ab,bc</t>
+  </si>
+  <si>
     <t xml:space="preserve">^ too many points for current renderer</t>
   </si>
   <si>
@@ -218,6 +224,9 @@
     <t xml:space="preserve">log2</t>
   </si>
   <si>
+    <t xml:space="preserve"> ab , bc </t>
+  </si>
+  <si>
     <t xml:space="preserve">feature_base</t>
   </si>
   <si>
@@ -230,6 +239,9 @@
     <t xml:space="preserve">log2/chunk-20210429_180100</t>
   </si>
   <si>
+    <t xml:space="preserve">,,,,</t>
+  </si>
+  <si>
     <t xml:space="preserve">generated_base</t>
   </si>
   <si>
@@ -240,6 +252,9 @@
   </si>
   <si>
     <t xml:space="preserve">log2/chunk-20210429_180200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,, bc ,,,</t>
   </si>
   <si>
     <t xml:space="preserve">other_base</t>
@@ -412,7 +427,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -440,11 +455,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -510,7 +520,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -531,7 +541,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,19 +549,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -638,11 +644,11 @@
   </sheetPr>
   <dimension ref="A1:Y530"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V13" activeCellId="0" sqref="V13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W11" activeCellId="0" sqref="W11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
@@ -768,64 +774,64 @@
         <v>24</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="R3" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="V3" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="W3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="E4" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>2</v>
@@ -834,49 +840,49 @@
         <v>24</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>192000</v>
@@ -885,17 +891,17 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G5" s="4"/>
       <c r="M5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>2</v>
@@ -906,35 +912,32 @@
         <v>2</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="W5" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="Y5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G6" s="4"/>
       <c r="M6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>2</v>
@@ -945,16 +948,16 @@
         <v>2</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>58</v>
+        <v>32</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="Y6" s="6"/>
     </row>
@@ -971,16 +974,16 @@
         <v>2</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V7" s="7" t="s">
-        <v>60</v>
+        <v>32</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="Y7" s="6"/>
     </row>
@@ -989,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>2</v>
@@ -998,66 +1001,66 @@
         <v>2</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="V8" s="7" t="s">
-        <v>32</v>
+        <v>65</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="Y8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="U9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="T9" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="V9" s="7" t="s">
-        <v>45</v>
+      <c r="V9" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="Y9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>2</v>
@@ -1067,25 +1070,25 @@
         <v>2</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="U10" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="V10" s="7" t="s">
-        <v>52</v>
+        <v>65</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="Y10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
@@ -1097,16 +1100,16 @@
         <v>2</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="V11" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y11" s="6"/>
     </row>
@@ -1121,25 +1124,25 @@
         <v>2</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="V12" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="V12" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
@@ -1157,7 +1160,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -1177,7 +1180,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>20</v>
@@ -1226,10 +1229,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>2</v>
@@ -1246,10 +1249,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
@@ -1280,11 +1283,11 @@
       <c r="V20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>83</v>
+      <c r="A21" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>2</v>
@@ -3436,216 +3439,216 @@
       <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="6" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="6" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="6" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="6" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="6" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="6" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="6" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="6" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="6" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="6" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="6" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="6" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="6" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="6" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="6" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="6" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="6" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="6" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="6" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="6" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="6" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="6" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="6" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="6" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Option --indent 1 to have multiline json conf export (for latter diffs)
</commit_message>
<xml_diff>
--- a/samples/tiny/config.xlsx
+++ b/samples/tiny/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="132">
   <si>
     <t xml:space="preserve">variables</t>
   </si>
@@ -128,142 +128,145 @@
     <t xml:space="preserve">20210429_180000</t>
   </si>
   <si>
+    <t xml:space="preserve">ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_base_cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/NOT-IMPLEMENT-YET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">band1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u_2sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sitetour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site Touristique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#9632ff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">four</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_180000-20210429_180400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log1/chunk-20210429_180100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_180100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_expected_sample_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">band2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192-64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first4min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 minutes taken at 18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log1/chunk-20210429_180200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_180200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_suffix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.WAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 minute at 18:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log1/chunk-20210429_180300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_180300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log1/chunk-20210429_181000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210429_181000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ab,bc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^ too many points for current renderer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_180000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ab , bc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature_base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^ pas utilisé, pourrait servir à choisir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_180100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,,,,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generated_base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./generated/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couleur etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_180200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,, bc ,,,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./other/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log2/chunk-20210429_180300</t>
+  </si>
+  <si>
     <t xml:space="preserve">rien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_base_cluster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/NOT-IMPLEMENT-YET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">u_2sec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sitetour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site Touristique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#9632ff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">four</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_180000-20210429_180400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log1/chunk-20210429_180100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_180100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_expected_sample_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">first4min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 minutes taken at 18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log1/chunk-20210429_180200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_180200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio_suffix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.WAV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 minute at 18:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log1/chunk-20210429_180300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_180300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log1/chunk-20210429_181000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20210429_181000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ab,bc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^ too many points for current renderer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log2/chunk-20210429_180000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ab , bc </t>
-  </si>
-  <si>
-    <t xml:space="preserve">feature_base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^ pas utilisé, pourrait servir à choisir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log2/chunk-20210429_180100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">,,,,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generated_base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./generated/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">couleur etc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log2/chunk-20210429_180200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">,, bc ,,,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other_base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./other/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log2/chunk-20210429_180300</t>
   </si>
   <si>
     <t xml:space="preserve">log2/chunk-20210429_181000</t>
@@ -644,8 +647,8 @@
   </sheetPr>
   <dimension ref="A1:Y530"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W11" activeCellId="0" sqref="W11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W4" activeCellId="0" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1109,7 +1112,7 @@
         <v>59</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="Y11" s="6"/>
     </row>
@@ -1124,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="U12" s="6" t="s">
         <v>65</v>
@@ -1133,13 +1136,13 @@
         <v>61</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="Y12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>31</v>
@@ -1160,7 +1163,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>0</v>
@@ -1180,7 +1183,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>20</v>
@@ -1229,10 +1232,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>2</v>
@@ -1249,10 +1252,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
@@ -1284,10 +1287,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>2</v>
@@ -3443,212 +3446,212 @@
   <sheetData>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Explore conditional coloring in (vue)chart.js
</commit_message>
<xml_diff>
--- a/samples/tiny/config.xlsx
+++ b/samples/tiny/config.xlsx
@@ -68,7 +68,7 @@
     <t xml:space="preserve">ranges</t>
   </si>
   <si>
-    <t xml:space="preserve">ranges_</t>
+    <t xml:space="preserve">ranges_ (utc)</t>
   </si>
   <si>
     <t xml:space="preserve">files (no suffix)</t>
@@ -647,8 +647,8 @@
   </sheetPr>
   <dimension ref="A1:Y530"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W4" activeCellId="0" sqref="W4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>